<commit_message>
update report  add interview summry #117
</commit_message>
<xml_diff>
--- a/production-idea/interview/interview-matome.xlsx
+++ b/production-idea/interview/interview-matome.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\namaz\Documents\ProjectP2016_F\production-idea\interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="70">
   <si>
     <t>ブックマークの数</t>
     <rPh sb="7" eb="8">
@@ -68,20 +68,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>使いたい</t>
-    <rPh sb="0" eb="1">
-      <t>ツカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>使いたくない</t>
-    <rPh sb="0" eb="1">
-      <t>ツカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>使う</t>
     <rPh sb="0" eb="1">
       <t>ツカ</t>
@@ -455,6 +441,117 @@
     <t>メディア系</t>
     <rPh sb="4" eb="5">
       <t>ケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>質問項目</t>
+    <rPh sb="0" eb="2">
+      <t>シツモン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>コウモク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このサービス使いたいか？</t>
+    <rPh sb="6" eb="7">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>使いたくないと答えた場合なぜ使いたくないのか</t>
+    <rPh sb="0" eb="1">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>コタ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SE</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>使う</t>
+    <rPh sb="0" eb="1">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BMして使わず忘れてしまう、整理したいけど時間がかかりそうでする気がなくなる</t>
+  </si>
+  <si>
+    <t>使っていない</t>
+    <rPh sb="0" eb="1">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ブックマークの中を整理するアプリ。自動で検索できる</t>
+  </si>
+  <si>
+    <t xml:space="preserve">便利だと思う。
+一回なら使うと思う。
+一回のために登録するのは面倒
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>使いたい</t>
+    <rPh sb="0" eb="1">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">検索するのが面倒
+手順が多くて手軽感があんまりない
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>もしもっと使いやすく出来たら便利だと思う。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>株とかやってる</t>
+    <rPh sb="0" eb="1">
+      <t>カブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ブックマークの中を整理するアプリ。検索したら勝手にまとめてくれる</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">便利だと思う。
+8割いらないやつだからまとめて削除出来たら使う
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>インポートエクスポートは面倒</t>
+  </si>
+  <si>
+    <t>質問項目２</t>
+    <rPh sb="0" eb="2">
+      <t>シツモン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>コウモク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -462,8 +559,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,21 +576,136 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="ＭＳ 明朝"/>
+      <family val="1"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -502,9 +714,51 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -786,333 +1040,546 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="7.875" customWidth="1"/>
-    <col min="3" max="3" width="17.125" customWidth="1"/>
-    <col min="4" max="4" width="16.25" customWidth="1"/>
-    <col min="5" max="5" width="17.875" customWidth="1"/>
-    <col min="6" max="6" width="19.75" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="19.875" customWidth="1"/>
-    <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="10" max="10" width="23.375" customWidth="1"/>
-    <col min="11" max="11" width="35.125" customWidth="1"/>
-    <col min="12" max="12" width="21.5" customWidth="1"/>
-    <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.08984375" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" customWidth="1"/>
+    <col min="7" max="7" width="15.90625" customWidth="1"/>
+    <col min="8" max="8" width="19.7265625" customWidth="1"/>
+    <col min="9" max="9" width="17.1796875" customWidth="1"/>
+    <col min="10" max="11" width="11.1796875" customWidth="1"/>
+    <col min="12" max="12" width="25" customWidth="1"/>
+    <col min="13" max="13" width="23.36328125" customWidth="1"/>
+    <col min="14" max="14" width="26.7265625" customWidth="1"/>
+    <col min="15" max="15" width="24.54296875" customWidth="1"/>
+    <col min="16" max="16" width="33.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="8"/>
+      <c r="C1" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="13"/>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D3" s="5">
+        <v>20</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="5">
+        <v>30</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D4" s="5">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5">
+        <v>80</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="L4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="1:16" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="6">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5">
+        <v>100</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6">
+        <v>3</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N5" s="5"/>
+      <c r="O5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" ht="149" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="6">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5">
+        <v>20</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="6">
+        <v>4</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="6">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5">
+        <v>20</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="F7" s="5">
+        <v>20</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="6">
+        <v>5</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="6">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5">
+        <v>20</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="5">
+        <v>30</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="6">
+        <v>6</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="6">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
-        <v>50</v>
+      <c r="C9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5">
+        <v>20</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="5">
+        <v>300</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6">
+        <v>7</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2">
+    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="6">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="5">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="5">
+        <v>30</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="J10" s="5"/>
+      <c r="K10" s="6">
+        <v>8</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="6">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="5">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="5">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
+      <c r="G11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6">
+        <v>9</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P11" s="5"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3">
+    <row r="12" spans="1:16" s="2" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="6">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="5">
+        <v>40</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="5">
+        <v>100</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6">
+        <v>10</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="2" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="6">
+        <v>11</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="5">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="5">
+        <v>200</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3">
-        <v>80</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B4">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>100</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B6">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="B7">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8">
-        <v>300</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>30</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>41</v>
-      </c>
-      <c r="J10" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" t="s">
-        <v>46</v>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6">
+        <v>11</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="L1:P1"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>